<commit_message>
top 20 ports and sssp for them
</commit_message>
<xml_diff>
--- a/ChinaRailway.xlsx
+++ b/ChinaRailway.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zi Hao\OneDrive\Documents\GitHub\PSAHackathon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACE9775-426F-4B6E-8749-E49222197D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DAD63E-5F9C-4875-93CC-EE1BDE588D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="12863" activeTab="1" xr2:uid="{647EEB31-6AD6-4954-ABF4-88A2238085C9}"/>
+    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="12863" xr2:uid="{647EEB31-6AD6-4954-ABF4-88A2238085C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="103">
   <si>
     <t>Origin/Destination</t>
   </si>
@@ -139,9 +140,6 @@
     <t>Kunming</t>
   </si>
   <si>
-    <t>Hong Kong</t>
-  </si>
-  <si>
     <t>Chongqing</t>
   </si>
   <si>
@@ -211,9 +209,6 @@
     <t>YANJI</t>
   </si>
   <si>
-    <t xml:space="preserve"> STATION 2</t>
-  </si>
-  <si>
     <t>STATION 1</t>
   </si>
   <si>
@@ -320,6 +315,60 @@
   </si>
   <si>
     <t>GUANGZHOU CONTAINER TERMINALS</t>
+  </si>
+  <si>
+    <t>STATION 2</t>
+  </si>
+  <si>
+    <t>PORT NAME</t>
+  </si>
+  <si>
+    <t>LOCATION OF PORT</t>
+  </si>
+  <si>
+    <t>NINGBO</t>
+  </si>
+  <si>
+    <t>QINGDAO GANG</t>
+  </si>
+  <si>
+    <t>SHANDONG</t>
+  </si>
+  <si>
+    <t>TIANJIN XIN GANG</t>
+  </si>
+  <si>
+    <t>TIANJIN</t>
+  </si>
+  <si>
+    <t>HONG KONG</t>
+  </si>
+  <si>
+    <t>DALIAN</t>
+  </si>
+  <si>
+    <t>LIANYUNGANG</t>
+  </si>
+  <si>
+    <t>JIANGSU</t>
+  </si>
+  <si>
+    <t>Jiangsu</t>
+  </si>
+  <si>
+    <t>Dalian</t>
+  </si>
+  <si>
+    <t>Fuzhou</t>
+  </si>
+  <si>
+    <t>Guangzhou</t>
+  </si>
+  <si>
+    <t>Tianjin</t>
+  </si>
+  <si>
+    <t>HongKong</t>
   </si>
 </sst>
 </file>
@@ -370,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -378,17 +427,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -724,10 +770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6EF9912-C81A-4D82-8F07-14F1482E0695}">
-  <dimension ref="B1:G38"/>
+  <dimension ref="B1:G43"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -743,32 +789,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>41</v>
+      <c r="F1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B2" s="4"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
@@ -975,7 +1021,7 @@
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B25" s="1" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="E25" s="1">
         <v>1</v>
@@ -986,7 +1032,7 @@
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B26" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E26" s="1">
         <v>1</v>
@@ -1000,7 +1046,7 @@
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B27" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E27" s="1">
         <v>1</v>
@@ -1011,7 +1057,7 @@
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B28" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E28" s="1">
         <v>1</v>
@@ -1022,7 +1068,7 @@
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B29" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F29" s="1">
         <v>1</v>
@@ -1030,7 +1076,7 @@
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B30" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F30" s="1">
         <v>1</v>
@@ -1038,7 +1084,7 @@
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B31" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F31" s="1">
         <v>1</v>
@@ -1046,7 +1092,7 @@
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B32" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F32" s="1">
         <v>1</v>
@@ -1054,7 +1100,7 @@
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B33" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F33" s="1">
         <v>1</v>
@@ -1062,7 +1108,7 @@
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B34" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F34" s="1">
         <v>1</v>
@@ -1070,7 +1116,7 @@
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B35" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F35" s="1">
         <v>1</v>
@@ -1078,7 +1124,7 @@
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B36" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F36" s="1">
         <v>1</v>
@@ -1086,7 +1132,7 @@
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B37" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F37" s="1">
         <v>1</v>
@@ -1094,10 +1140,35 @@
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B38" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F38" s="1">
         <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B39" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B40" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B41" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B42" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B43" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1116,10 +1187,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CFBD139-7FAB-46C1-B54E-77AD1313B73A}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:B17"/>
+    <sheetView zoomScale="58" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1134,33 +1205,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="5"/>
-      <c r="B1" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="A1"/>
+      <c r="B1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>81</v>
       </c>
+      <c r="F1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="5"/>
+      <c r="A2"/>
       <c r="B2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="D2" s="2">
         <v>49</v>
@@ -1180,10 +1251,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="D3" s="2">
         <v>43</v>
@@ -1200,10 +1271,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="D4" s="2">
         <v>86</v>
@@ -1220,10 +1291,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="2">
         <v>76</v>
@@ -1240,10 +1311,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="D6" s="2">
         <v>70</v>
@@ -1260,10 +1331,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" s="2">
         <v>240</v>
@@ -1280,10 +1351,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" s="2">
         <v>135</v>
@@ -1300,10 +1371,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D9" s="2">
         <v>230</v>
@@ -1320,10 +1391,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D10" s="2">
         <v>25</v>
@@ -1340,10 +1411,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B11" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D11" s="2">
         <v>58</v>
@@ -1360,10 +1431,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B12" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D12" s="2">
         <v>63</v>
@@ -1380,10 +1451,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B13" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D13" s="2">
         <v>60</v>
@@ -1400,10 +1471,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B14" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D14" s="2">
         <v>40</v>
@@ -1420,10 +1491,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B15" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
@@ -1440,10 +1511,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B16" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D16" s="2">
         <v>120</v>
@@ -1460,10 +1531,10 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B17" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D17" s="2">
         <v>190</v>
@@ -1480,10 +1551,10 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B18" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D18" s="2">
         <v>75</v>
@@ -1500,10 +1571,10 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B19" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D19" s="2">
         <v>216</v>
@@ -1520,10 +1591,10 @@
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="D20" s="2">
         <v>132</v>
@@ -1540,10 +1611,10 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="D21" s="2">
         <v>60</v>
@@ -1560,10 +1631,10 @@
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B22" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D22" s="2">
         <v>78</v>
@@ -1580,10 +1651,10 @@
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B23" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D23" s="2">
         <v>86</v>
@@ -1600,10 +1671,10 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="D24" s="2">
         <v>150</v>
@@ -1620,10 +1691,10 @@
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B25" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D25" s="2">
         <v>86</v>
@@ -1640,10 +1711,10 @@
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B26" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D26" s="2">
         <v>32</v>
@@ -1660,10 +1731,10 @@
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B27" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D27" s="2">
         <v>72</v>
@@ -1680,10 +1751,10 @@
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B28" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D28" s="2">
         <v>66</v>
@@ -1700,10 +1771,10 @@
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B29" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D29" s="2">
         <v>162</v>
@@ -1720,10 +1791,10 @@
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B30" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="D30" s="2">
         <v>120</v>
@@ -1740,10 +1811,10 @@
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B31" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D31" s="2">
         <v>70</v>
@@ -1760,10 +1831,10 @@
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B32" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D32" s="2">
         <v>134</v>
@@ -1780,10 +1851,10 @@
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B33" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D33" s="2">
         <v>340</v>
@@ -1800,10 +1871,10 @@
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B34" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D34" s="2">
         <v>200</v>
@@ -1820,10 +1891,10 @@
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B35" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D35" s="2">
         <v>30</v>
@@ -1840,10 +1911,10 @@
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B36" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D36" s="2">
         <v>90</v>
@@ -1860,10 +1931,10 @@
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B37" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D37" s="2">
         <v>280</v>
@@ -1880,10 +1951,10 @@
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B38" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D38" s="2">
         <v>320</v>
@@ -1900,10 +1971,10 @@
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B39" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D39" s="2">
         <v>240</v>
@@ -1920,10 +1991,10 @@
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B40" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D40" s="2">
         <v>350</v>
@@ -1938,10 +2009,118 @@
         <v>1750</v>
       </c>
     </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B41" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0</v>
+      </c>
+      <c r="E41" s="2">
+        <v>0</v>
+      </c>
+      <c r="F41" s="2">
+        <v>6.6666666670000003</v>
+      </c>
+      <c r="G41" s="2">
+        <v>500</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:A2"/>
-  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57256FE3-BBA5-4464-B436-0B9B7A38C57C}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.06640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>